<commit_message>
updated 30 May Code
</commit_message>
<xml_diff>
--- a/Capsulecrm/src/main/resources/InputData.xlsx
+++ b/Capsulecrm/src/main/resources/InputData.xlsx
@@ -9,12 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4635" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4635"/>
   </bookViews>
   <sheets>
     <sheet name="AddPerson" sheetId="1" r:id="rId1"/>
     <sheet name="AccountSettings" sheetId="2" r:id="rId2"/>
     <sheet name="Users" sheetId="3" r:id="rId3"/>
+    <sheet name="Opportunities" sheetId="4" r:id="rId4"/>
+    <sheet name="Track" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -26,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="55">
   <si>
     <t>FirstName</t>
   </si>
@@ -130,25 +132,67 @@
     <t>UserName</t>
   </si>
   <si>
-    <t>Shubham</t>
-  </si>
-  <si>
-    <t>Joshi</t>
-  </si>
-  <si>
-    <t>shubhamjoshi12@yahoo.in</t>
-  </si>
-  <si>
-    <t>shujoshi</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nayan </t>
-  </si>
-  <si>
-    <t>nayanjoshi@yahoo.in</t>
-  </si>
-  <si>
-    <t>nayjoshi</t>
+    <t>jon</t>
+  </si>
+  <si>
+    <t>snow</t>
+  </si>
+  <si>
+    <t>jon@snowgmail.com</t>
+  </si>
+  <si>
+    <t>snowbaba</t>
+  </si>
+  <si>
+    <t>MileStoneName</t>
+  </si>
+  <si>
+    <t>MileStoneDescription</t>
+  </si>
+  <si>
+    <t>ProbabilityofWinning</t>
+  </si>
+  <si>
+    <t>DaysUntilStale</t>
+  </si>
+  <si>
+    <t>TrackName</t>
+  </si>
+  <si>
+    <t>TagName</t>
+  </si>
+  <si>
+    <t>TaskDescription</t>
+  </si>
+  <si>
+    <t>Category</t>
+  </si>
+  <si>
+    <t>Due</t>
+  </si>
+  <si>
+    <t>Career</t>
+  </si>
+  <si>
+    <t>Call</t>
+  </si>
+  <si>
+    <t>Scenario</t>
+  </si>
+  <si>
+    <t>Scenario Outline</t>
+  </si>
+  <si>
+    <t>100</t>
+  </si>
+  <si>
+    <t>999</t>
+  </si>
+  <si>
+    <t>Asssam</t>
+  </si>
+  <si>
+    <t>Mission Assam</t>
   </si>
 </sst>
 </file>
@@ -205,12 +249,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -494,8 +539,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -550,8 +595,8 @@
       <c r="E2" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="1">
-        <v>9999999999</v>
+      <c r="F2" s="5">
+        <v>5063255478</v>
       </c>
       <c r="G2" t="s">
         <v>11</v>
@@ -571,7 +616,7 @@
   <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -592,10 +637,10 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>16</v>
       </c>
     </row>
@@ -608,90 +653,90 @@
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="1" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="1" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="1" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="1" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="1" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="1" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
+      <c r="A10" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="1" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
+      <c r="A11" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="2" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
+      <c r="A12" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="1" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
+      <c r="A13" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B13" s="1" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
+      <c r="A14" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="B14" s="2" t="s">
         <v>21</v>
       </c>
     </row>
@@ -702,10 +747,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -737,32 +782,121 @@
       <c r="B2" t="s">
         <v>35</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="3" t="s">
         <v>36</v>
       </c>
       <c r="D2" t="s">
         <v>37</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>38</v>
-      </c>
-      <c r="B3" t="s">
-        <v>35</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="D3" t="s">
-        <v>40</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1"/>
-    <hyperlink ref="C3" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C2">
+        <v>75</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="24.140625" customWidth="1"/>
+    <col min="2" max="2" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>